<commit_message>
Updated after second round comment resolution
</commit_message>
<xml_diff>
--- a/RESTful_ATNA/ITI_RESTful_ATNA_Comments_Consolidated.xlsx
+++ b/RESTful_ATNA/ITI_RESTful_ATNA_Comments_Consolidated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregorio Canal\Google Drive\IHE\ITI\Add RESTFULL Feed to ATNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBFBE75-E07A-4A65-9E5E-78E2AC2AF838}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C43D1FE-687E-4E8A-AE97-936DEA3CDFF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="177">
   <si>
     <t>Priority</t>
   </si>
@@ -1131,9 +1131,6 @@
     </r>
   </si>
   <si>
-    <t>See changes</t>
-  </si>
-  <si>
     <t>Fixed</t>
   </si>
   <si>
@@ -1147,9 +1144,6 @@
   </si>
   <si>
     <t xml:space="preserve">agree, 404 should be returned if the url used point to a type of resource not present in the server, not related to to the content. </t>
-  </si>
-  <si>
-    <t>ok, to not use 404, but it is 400 ok? Right now the client could send other type of resource in the bundle we only require that there is at least one AuditEvent resource. If we were more strict i would be ok with a 400.. What to do? Change request requirment?</t>
   </si>
   <si>
     <t>I'am more for the new option. It is a breaking change but maybe a note for future integration statment that says that IG released before  date XX support by default the syslog option</t>
@@ -1258,9 +1252,6 @@
   </si>
   <si>
     <t>Generl</t>
-  </si>
-  <si>
-    <t>Duplicate</t>
   </si>
   <si>
     <t>see line 32</t>
@@ -1336,12 +1327,6 @@
     <t>CP-1145 integrated. Do we need to add text for compatibility of options? CP-1145 is the only CP in final text for now..</t>
   </si>
   <si>
-    <t>To do</t>
-  </si>
-  <si>
-    <t>Can you point us to the right CP?</t>
-  </si>
-  <si>
     <t>FIxed</t>
   </si>
   <si>
@@ -1353,6 +1338,18 @@
   </si>
   <si>
     <t>added an open issue, for PRI that is the only one not addressed, but it will be R5</t>
+  </si>
+  <si>
+    <t>added a link to the FHIR spec in order to see what to do with status codes in case of failures.</t>
+  </si>
+  <si>
+    <t>removed ordering sentence</t>
+  </si>
+  <si>
+    <t>Later review will try to fix this</t>
+  </si>
+  <si>
+    <t>Deferred</t>
   </si>
 </sst>
 </file>
@@ -1958,10 +1955,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2064,7 +2062,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="303.60000000000002" x14ac:dyDescent="0.3">
@@ -2096,7 +2094,7 @@
         <v>130</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
@@ -2126,7 +2124,7 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
@@ -2156,7 +2154,7 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
@@ -2185,10 +2183,10 @@
         <v>9</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="198" x14ac:dyDescent="0.3">
@@ -2217,10 +2215,10 @@
         <v>10</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
@@ -2249,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2282,7 +2280,7 @@
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
@@ -2312,7 +2310,7 @@
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
@@ -2338,7 +2336,7 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="66" x14ac:dyDescent="0.3">
@@ -2368,7 +2366,7 @@
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2398,7 +2396,7 @@
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="105.6" x14ac:dyDescent="0.3">
@@ -2428,7 +2426,7 @@
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2456,7 +2454,7 @@
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="108.6" x14ac:dyDescent="0.3">
@@ -2483,7 +2481,7 @@
         <v>8</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>131</v>
@@ -2515,10 +2513,10 @@
         <v>8</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="118.8" x14ac:dyDescent="0.3">
@@ -2547,10 +2545,10 @@
         <v>9</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
@@ -2580,7 +2578,7 @@
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
@@ -2609,7 +2607,7 @@
         <v>8</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>131</v>
@@ -2642,10 +2640,10 @@
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="85.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -2666,9 +2664,11 @@
       <c r="H26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="J26" s="7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -2698,7 +2698,7 @@
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
@@ -2753,7 +2753,7 @@
         <v>9</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J29" s="23" t="s">
         <v>131</v>
@@ -2776,17 +2776,17 @@
         <v>1025</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
@@ -2813,13 +2813,13 @@
         <v>8</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="118.8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>123</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>8</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>131</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="33" spans="1:10" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>58</v>
@@ -2860,30 +2860,30 @@
         <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E33" s="12">
         <v>795</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>58</v>
@@ -2892,22 +2892,22 @@
         <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E34" s="12">
         <v>1065</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>131</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="35" spans="1:10" ht="66" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>58</v>
@@ -2924,30 +2924,30 @@
         <v>111</v>
       </c>
       <c r="D35" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E35" s="12">
         <v>1245</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>58</v>
@@ -2956,30 +2956,30 @@
         <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E36" s="12">
         <v>1260</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>58</v>
@@ -2988,20 +2988,20 @@
         <v>111</v>
       </c>
       <c r="D37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E37" s="12">
         <v>651</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="21" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>131</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="38" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>58</v>
@@ -3024,22 +3024,22 @@
         <v>1295</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>58</v>
@@ -3054,49 +3054,49 @@
         <v>1302</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -3260,7 +3260,13 @@
       <c r="H56" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:J40" xr:uid="{3E9B721A-4FCD-4100-9841-9ADC0EB70ECC}"/>
+  <autoFilter ref="A5:J40" xr:uid="{3E9B721A-4FCD-4100-9841-9ADC0EB70ECC}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Fixed"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A1:I1"/>

</xml_diff>